<commit_message>
Avvisi frontend desktop completed
</commit_message>
<xml_diff>
--- a/completezza funzionale_frontend.xlsx
+++ b/completezza funzionale_frontend.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salvc\Desktop\Ratatouille23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76E3E3E-393F-4CE0-9D81-96874B537FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1024E9-363D-402D-96C6-5F6260EB71A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Funzionalità #1</t>
   </si>
@@ -114,7 +114,10 @@
     <t>GestioneProfilo</t>
   </si>
   <si>
-    <t>Finito</t>
+    <t>Login completato</t>
+  </si>
+  <si>
+    <t>SignUp completato</t>
   </si>
 </sst>
 </file>
@@ -590,7 +593,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +774,9 @@
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -792,7 +797,6 @@
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">

</xml_diff>

<commit_message>
Bug fix nella descrizione
Gestione del token
Pagina avvisi migliorata UI
Some changes signed in todotree.txt
</commit_message>
<xml_diff>
--- a/completezza funzionale_frontend.xlsx
+++ b/completezza funzionale_frontend.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salvc\Desktop\Ratatouille23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1024E9-363D-402D-96C6-5F6260EB71A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4957F6E8-B1B7-4B4D-AA96-7CB1B46F4E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>Funzionalità #1</t>
   </si>
@@ -84,12 +84,6 @@
     <t>STEP</t>
   </si>
   <si>
-    <t>RESPONSABILE:</t>
-  </si>
-  <si>
-    <t>DISEGNO XML PAGINE STATICHE</t>
-  </si>
-  <si>
     <t>Login/SignUp</t>
   </si>
   <si>
@@ -102,22 +96,85 @@
     <t>Risorse Umane</t>
   </si>
   <si>
-    <t>Alfredo</t>
-  </si>
-  <si>
-    <t>Cristian</t>
-  </si>
-  <si>
     <t>PersonalizzazioneRistorante</t>
   </si>
   <si>
     <t>GestioneProfilo</t>
   </si>
   <si>
-    <t>Login completato</t>
-  </si>
-  <si>
-    <t>SignUp completato</t>
+    <t xml:space="preserve">Login </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SignUp </t>
+  </si>
+  <si>
+    <t>Visualizzazione piatti (VP)</t>
+  </si>
+  <si>
+    <t>Struttura FXML statico</t>
+  </si>
+  <si>
+    <t>Struttura FXML statico delle pagine</t>
+  </si>
+  <si>
+    <t>Struttura FXML statico della pagina</t>
+  </si>
+  <si>
+    <t>VP : aggiunta card visuale dinamica</t>
+  </si>
+  <si>
+    <t>VP : aggiunta funzionalità bottoni di cancellazione piatto</t>
+  </si>
+  <si>
+    <t>VP : aggiunta funzionalità ricerca piatto</t>
+  </si>
+  <si>
+    <t>Ordina menu (OM)</t>
+  </si>
+  <si>
+    <t>OM : Aggiunta funzionalità scelta ordinamento</t>
+  </si>
+  <si>
+    <t>OM : Aggiunta funzionalità visualizza menu già presente</t>
+  </si>
+  <si>
+    <t>OM : Aggiunta funzionalità reset categoria</t>
+  </si>
+  <si>
+    <t>Modifica Piatto (MP)</t>
+  </si>
+  <si>
+    <t>MP: Inserimento dati e richieste</t>
+  </si>
+  <si>
+    <t>Aggiunta card visuale dinamica</t>
+  </si>
+  <si>
+    <t>Aggiunta funzionalità scrittura avviso</t>
+  </si>
+  <si>
+    <t>Aggiunta funzionalità cancellazione avviso</t>
+  </si>
+  <si>
+    <t>Aggiunta affordance</t>
+  </si>
+  <si>
+    <t>Aggiunta affordance a tutto il menu</t>
+  </si>
+  <si>
+    <t>Disegno xml pagina dispensa</t>
+  </si>
+  <si>
+    <t>Dispensa</t>
+  </si>
+  <si>
+    <t>Aggiungi Piatto(AP)</t>
+  </si>
+  <si>
+    <t>AP: Inserimento dati e richieste</t>
+  </si>
+  <si>
+    <t>AP: Inserimento automompletamento con opendata</t>
   </si>
 </sst>
 </file>
@@ -163,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -174,6 +231,19 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -184,13 +254,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -310,8 +381,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF704CF4-E7A5-49C9-AEA8-4A06D27827BD}" name="Tabella13" displayName="Tabella13" ref="A16:I28" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A16:I28" xr:uid="{CF704CF4-E7A5-49C9-AEA8-4A06D27827BD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF704CF4-E7A5-49C9-AEA8-4A06D27827BD}" name="Tabella13" displayName="Tabella13" ref="A16:I33" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A16:I33" xr:uid="{CF704CF4-E7A5-49C9-AEA8-4A06D27827BD}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{48A01EBC-F6CD-45F2-B0F4-73331B15F64E}" name="STEP" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{0EED48F9-10EE-46F5-8E1D-26B9841F7CBD}" name="Funzionalità #1"/>
@@ -593,14 +664,15 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="45.28515625" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
-    <col min="4" max="9" width="45.28515625" customWidth="1"/>
+    <col min="4" max="4" width="57" customWidth="1"/>
+    <col min="5" max="9" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -635,7 +707,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -649,11 +721,17 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -698,9 +776,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -742,22 +818,22 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -769,82 +845,191 @@
       <c r="B18" t="s">
         <v>29</v>
       </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>30</v>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E37" s="1"/>
     </row>
   </sheetData>

</xml_diff>